<commit_message>
updated as of Jan 2024, just starting work on DOC data processing
</commit_message>
<xml_diff>
--- a/data/Kirby_FL2/fl2_meta.xlsx
+++ b/data/Kirby_FL2/fl2_meta.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Dropbox\Kirby_priming\DOC_priming\data\Kirby_FL2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71D270AB-3FD0-4608-A38D-55C3EDA0160D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF8E3BE9-07CE-4F9E-8A90-A4006A39130C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E89BA982-13AD-4E3C-8C1C-ECE45B6BE5F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fl2_meta" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
   <si>
     <t>Syringe</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>70B</t>
   </si>
 </sst>
 </file>
@@ -568,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A6C5FB-ADB8-4EEF-9585-013C56BD011C}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,7 +641,7 @@
         <v>0.60486111111111118</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F17" si="0">26.74*0.033421</f>
+        <f t="shared" ref="F3:F16" si="0">26.74*0.033421</f>
         <v>0.89367753999999988</v>
       </c>
     </row>
@@ -1133,7 +1136,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1325,7 +1328,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1517,7 +1520,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1709,7 +1712,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -1901,7 +1904,7 @@
         <v>51</v>
       </c>
       <c r="B58">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -2377,8 +2380,8 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>70</v>
+      <c r="A78" t="s">
+        <v>59</v>
       </c>
       <c r="B78">
         <v>8</v>

</xml_diff>